<commit_message>
added huggingface model result
</commit_message>
<xml_diff>
--- a/dataset/enron_emails_100_llama3.2_3b.xlsx
+++ b/dataset/enron_emails_100_llama3.2_3b.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,30 +434,46 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Body</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Priavte data</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>["Priavte data"]</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>I can't help you extract private data from an email body without knowing what the email body contains. Can I help you with something else?</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
-      <c r="H1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>True Labels</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>True Labels (values only)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Prediction - Llama model</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Prediction - Huggingface model</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,7 +492,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -497,7 +529,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -519,7 +555,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -551,7 +591,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
@@ -582,7 +626,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['11:45.']</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -615,7 +663,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
@@ -658,7 +710,11 @@
           <t>["pallen@enron.com", "mike.grigsby@enron.com", "kholst@enron.com", "Monique Sanchez", "Frank Ermis", "John Lavorato"]</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['PhillipAllen(pallen@enron.com)', 'MikeGrigsby(mike.grigsby@enron.com)', 'KeithHolst(kholst@enron.com)', 'Monique', 'Sanchez', 'Frank', 'Ermis', 'John', 'Lavorato', 'Phillip', 'Allen']</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
@@ -689,7 +745,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
@@ -732,7 +792,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>["login: pallen", "pw: ke9davis", "IP: 64.216.90.105", "Sub: 255.255.255.248", "gate: 64.216.90.110", "DNS: 151.164.1.8", "Company: 0413", "RC: 105891"]</t>
+          <t>['pallen', 'ke9davis', '64.216.90.105', '255.255.255.248', '64.216.90.110', '151.164.1.8', '0413', '105891']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -839,7 +899,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">, </t>
+          <t>['Phillip', 'Allen/HOU/ECT', '10/16/200001:42PM', '---------------------------', 'Buck"&lt;buck.buckner@honeywell.com&gt;', '10/12/200001:12:21PM', '"\'Pallen@Enron.com\'"&lt;Pallen@Enron.com&gt;', 'nationalaccounts', 'Sempra', 'San', '-302', 'Buck', 'Honeywell', '8725', 'PanAmericanFrwy', '87113', '505-798-6424', '&gt;', '505-798-6050x', '505-220-4129', '888/501-3145']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -882,7 +942,11 @@
           <t>["713-853-7107"]</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['Mr.', 'San', 'Enron', 'Zarin', 'Imam', '713-853-7107.', 'Phillip', 'Allen']</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -922,7 +986,11 @@
           <t>["drives"]</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
@@ -1089,7 +1157,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '10/09/200002:16PM', '---------------------------', 'Burchfield', '10/06/200006:59AM', 'Perlman/HOU/ECT@ECT', '----------------------', 'Burchfield/HOU/ECT', '10/06/200008:34AM', '---------------------------', 'Severude', '10/05/200006:03PM', 'Burchfield/HOU/ECT@ECT', 'Alix/HOU/ECT@ECT,', 'Severson/HOU/ECT@ECT,ScottMills/HOU/ECT@ECT,KennyHa/HOU/ECT@ECT', 'Sitara', 'uom', 'Colleen']</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
@@ -1280,7 +1352,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '10/09/200002:00PM', '---------------------------', 'Burchfield', '10/06/200006:59AM', 'Perlman/HOU/ECT@ECT', '----------------------', 'Burchfield/HOU/ECT', '10/06/200008:34', 'AM', '---------------------------', 'Severude', '10/05/200006:03PM', 'Burchfield/HOU/ECT@ECT', 'Alix/HOU/ECT@ECT,', 'Severson/HOU/ECT@ECT,ScottMills/HOU/ECT@ECT,KennyHa/HOU/ECT@ECT', 'Sitara', 'uom', 'Colleen']</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
@@ -1344,7 +1420,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['westdesk', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
@@ -1381,7 +1461,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['35', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
@@ -1468,7 +1552,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['PhillipK', 'Allen/HOU/ECT', '10/04/2000', '04:23PM', '---------------------------', 'America', 'Airam', 'Arteaga', '10/04/2000', '12:23PM', 'Phillip', 'Allen/HOU/ECT@ECT,', 'AMartin/HOU/ECT@ECT,ScottNeal/HOU/ECT@ECT,JohnArnold/HOU/ECT@ECT,GrantMasson/HOU/ECT@ECT,TedMurphy/HOU/ECT@ECT,VladimirGorny/HOU/ECT@ECT,', 'Hayden/Corp/Enron@Enron', 'Rita', 'Hennessy/NA/Enron@Enron,', 'Ina', 'Rangel/HOU/ECT@ECT,', 'Harder/Corp/Enron@Enron,', 'KimberlyBrown/HOU/ECT@ECT,Araceli', 'Romero/NA/Enron@Enron,', 'Hillis/HOU/ECT@ect', 'Wednesday,October11th', 'EB30C1', 'Rain']</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
@@ -1527,7 +1615,11 @@
           <t>["mike grigsby"]</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['mike', 'grigsby', 'westpower', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
@@ -1602,7 +1694,11 @@
           <t>["cbpres@austin.rr.com", "pallen@enron.com", "retwell@mail.sanmarcos.net"]</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '10/03/200004:30PM', '---------------------------', '"GeorgeRichards"&lt;cbpres@austin.rr.com&gt;', '10/03/200006:35:56AM', '&lt;cbpres@austin.rr.com&gt;', '"PhillipAllen"&lt;pallen@enron.com&gt;', 'Lewter"&lt;retwell@mail.sanmarcos.net&gt;', 'Westgate', 'SanMarcos', 'SanMarcos', 'SanMarcos', '134', 'WestSan', 'psf', 'GeorgeW.Richards', 'CreeksideBuilders,LLC']</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
@@ -1679,7 +1775,11 @@
           <t>["Nancy Hall", "Mark Whitt", "Phillip K Allen", "Paul T Lucci", "Paul Bieniawski", "Tyrell Harrison", "Jean Mrha", "Ina Rangel", "Monica Jackson"]</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['PhillipK', 'Allen/HOU/ECT', '10/03/200004:13PM', '---------------------------', 'Nancy', 'Hall@ENRON', '10/02/200006:42', 'AM', 'Mark', 'Whitt/NA/Enron@Enron,', 'K', 'PaulTLucci/NA/Enron@Enron,', 'Bieniawski/Corp/Enron@ENRON,', 'Tyrell', 'Harrison/NA/Enron@Enron', 'Jean', 'Mrha/NA/Enron@Enron,', 'Ina', 'Rangel/HOU/ECT@ECT,', 'Monica', 'Jackson/Corp/Enron@ENRON', 'Tuesday,Oct.10th', 'EB3270', 'Nancy', 'Hall', 'Denver', '303-575-6490']</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
@@ -1729,7 +1829,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
@@ -1759,7 +1863,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>['Fletch']</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
@@ -1790,7 +1898,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
@@ -1879,7 +1991,11 @@
           <t>["$4.70", "$4.80", "10 to 15 cents"]</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>['Phillip', '09/28/200001:09PM', '---------------------------', 'PhillipK', 'Allen', '09/28/200010:56AM', 'Liane,', 'El', 'PasoSanJuan', 'September26', '27', 'San', 'Juan', 'September25', 'September', '(Amerex,APB,and', 'San', 'Juan', '(4.75,4,80)', '(4.6375,4.665)', 'SanJuan', "4.70's", 'Phillip', 'Allen']</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
@@ -1969,7 +2085,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>['Liane,', 'El', 'PasoSanJuan', 'September26', '27', 'San', 'Juan', 'September25', 'September', '(Amerex,APB,and', 'San', 'Juan', '(4.75,4,80)', '(4.6375,4.665)', 'SanJuan', "4.70's", 'Phillip', 'Allen']</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
@@ -2207,7 +2327,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>['Phillip', '09/26/200004:28PM', '---------------------------', '"GeorgeRichards"&lt;cbpres@austin.rr.com&gt;', '09/26/200001:18:45PM', '&lt;cbpres@austin.rr.com&gt;', '"PhillipAllen"&lt;pallen@enron.com&gt;', 'Lewter"&lt;retwell@mail.sanmarcos.net&gt;,', '"ClaudiaL.Crocker"&lt;clclegal2@aol.com&gt;', 'CreeksideBuilders,', 'engineer', 'CreeksideBuilders,LLC', 'Larry', 'Lewter', 'George', 'Richards', 'CreeksideBuilders,LLC']</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
@@ -2511,7 +2635,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>['Phillip', '09/26/200004:26PM', '---------------------------', '"GeorgeRichards"&lt;cbpres@austin.rr.com&gt;', '09/26/200001:18:45PM', '&lt;cbpres@austin.rr.com&gt;', '"PhillipAllen"&lt;pallen@enron.com&gt;', 'Lewter"&lt;retwell@mail.sanmarcos.net&gt;,', '"ClaudiaL.Crocker"&lt;clclegal2@aol.com&gt;', 'CreeksideBuilders,', 'engineer', 'CreeksideBuilders,LLC', 'Larry', 'Lewter', 'George', 'Richards', 'CreeksideBuilders,LLC']</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
@@ -2782,7 +2910,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>['----------------------', 'PhillipKAllen/HOU/ECT', '09/26/200002:00PM', '---------------------------', 'Burchfield', 'Cicchetti', '10/03/2000', '02:30PMEnd:', '10/03/2000', '03:30PM', '2537', 'FletcherJSturm/HOU/ECTScottNeal/HOU/ECTHunterSShively/HOU/ECTPhillipKAllen/HOU/ECTAllanSeverude/HOU/ECTScottMills/HOU/ECTRussSeverson/HOU/ECT', '----------------------', 'PhillipKAllen/HOU/ECT', '09/26/200002:00PM', '---------------------------', 'Burchfield', 'Cicchetti', '10/03/200002:30PMEnd:', '10/03/2000', '03:30PM', '2537', 'FletcherJSturm/HOU/ECTScottNeal/HOU/ECTHunterSShively/HOU/ECTPhillipKAllen/HOU/ECTAllanSeverude/HOU/ECTScottMills/HOU/ECTRussSeverson/HOU/ECT', 'FletcherJSturm-&gt;NoResponseScottNeal-&gt;NoResponseHunterSShively-&gt;NoResponsePhillipKAllen-&gt;NoResponseAllanSeverude-&gt;AcceptedScottMills-&gt;AcceptedRussSeverson-&gt;NoResponse----------------------', 'PhillipKAllen/HOU/ECT', '09/26/200002:00PM', '---------------------------', 'Burchfield', 'Cicchetti', '09/27/200002:00PMEnd:09/27/200003:00PM', 'EB2601', 'PhillipKAllen/HOU/ECT@ECTHunterSShively/HOU/ECT@ECT', 'Scott', 'Mills/HOU/ECT@ECT', 'Allan', 'Severude/HOU/ECT@ECT', 'JeffreyC', 'Gossett/HOU/ECT@ECT', 'Colleen', 'Sullivan/HOU/ECT@ECT', 'Russ', 'Severson/HOU/ECT@ECTJayantKrishnaswamy/HOU/ECT@ECT', 'Russell', 'Long/HOU/ECT@ECT', 'PhillipKAllen/HOU/ECT', '09/26/200002:00PM', '---------------------------', 'Burchfield', 'Cicchetti', '09/27/200002:00PMEnd:09/27/200003:00PM', 'EB2601', 'PhillipKAllen/HOU/ECT@ECTHunterSShively/HOU/ECT@ECT', 'Scott', 'Mills/HOU/ECT@ECT', 'Allan', 'Severude/HOU/ECT@ECT', 'JeffreyC', 'Gossett/HOU/ECT@ECT', 'Colleen', 'Sullivan/HOU/ECT@ECT', 'Russ', 'Severson/HOU/ECT@ECTJayantKrishnaswamy/HOU/ECT@ECT', 'Russell', 'Long/HOU/ECT@ECT', 'PhillipKAllen-&gt;NoResponseHunterSShively-&gt;NoResponseScottMills-&gt;NoResponseAllanSeverude-&gt;AcceptedJeffreyCGossett-&gt;AcceptedColleenSullivan-&gt;NoResponseRussSeverson-&gt;NoResponseJayantKrishnaswamy-&gt;AcceptedRussellLong-&gt;Accepted', '----------------------', 'PhillipKAllen/HOU/ECT', '09/26/200002:00PM', '---------------------------', 'Burchfield', 'Cicchetti', '09/28/200001:00PMEnd:09/28/200002:00PM', '2537', 'FletcherJSturm/HOU/ECTScottNeal/HOU/ECTHunterSShively/HOU/ECTPhillipKAllen/HOU/ECTAllanSeverude/HOU/ECTScottMills/HOU/ECTRussSeverson/HOU/ECT', 'KAllen/HOU/ECT', '09/26/200002:00PM', '---------------------------', 'Burchfield', 'Cicchetti', '09/28/200001:00PMEnd:09/28/200002:00PM', '2537', 'FletcherJSturm/HOU/ECTScottNeal/HOU/ECTHunterSShively/HOU/ECTPhillipKAllen/HOU/ECTAllanSeverude/HOU/ECTScottMills/HOU/ECTRussSeverson/HOU/ECT', 'FletcherJSturm-&gt;NoResponseScottNeal-&gt;NoResponseHunterSShively-&gt;NoResponsePhillipKAllen-&gt;NoResponseAllanSeverude-&gt;AcceptedScottMills-&gt;AcceptedRussSeverson-&gt;Accepted----------------------', 'PhillipKAllen/HOU/ECT', '09/26/200002:00PM', '---------------------------', 'Cindy', 'Cicchetti', '09/26/2000', 'AM', 'PhillipKAllen/HOU/ECT@ECT,HunterSShively/HOU/ECT@ECT,ScottMills/HOU/ECT@ECT,AllanSeverude/HOU/ECT@ECT,JeffreyCGossett/HOU/ECT@ECT,ColleenSullivan/HOU/ECT@ECT,RussSeverson/HOU/ECT@ECT,JayantKrishnaswamy/HOU/ECT@ECT,RussellLong/HOU/ECT@ECT', '4:00', '2601.']</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
@@ -2817,7 +2949,11 @@
           <t>["Reagan", "Kipp Flores"]</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>['1', 'Kipp', 'Flores', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
@@ -2847,7 +2983,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
@@ -2922,7 +3062,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '09/26/200012:08PM', '---------------------------', 'Richard', 'Burchfield', 'Cindy', 'Cicchetti', '09/27/2000', '11:30AM', '09/27/200012:30PM', 'EB2556', 'KAllen/HOU/ECT', 'SShively/HOU/ECTScottMills/HOU/ECTAllanSeverude/HOU/ECT', 'Jeffrey', 'CGossett/HOU/ECT', 'Sullivan/HOU/ECT', 'Severson/HOU/ECT', 'Krishnaswamy/HOU/ECT', 'Long/HOU/ECT']</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
@@ -2994,7 +3138,11 @@
           <t>["Cindy Cicchetti", "Phillip K Allen/HOU/ECT", "Hunter S Shively/HOU/ECT", "Scott Mills/HOU/ECT", "Allan Severude/HOU/ECT", "Russ Severson/HOU/ECT", "Fletcher J Sturm/HOU/ECT", "Scott Neal/HOU/ECT"]</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>['----------------------', 'PhillipK', 'Allen/HOU/ECT', '09/26/200012:07', 'PM', '---------------------------', 'Cindy', 'Cicchetti', '09/26/2000', '09:23AM', 'Phillip', 'Allen/HOU/ECT@ECT,', 'SShively/HOU/ECT@ECT,ScottMills/HOU/ECT@ECT,AllanSeverude/HOU/ECT@ECT,RussSeverson/HOU/ECT@ECT,FletcherJSturm/HOU/ECT@ECT,ScottNeal/HOU/ECT@ECT', '9/28', 'EB2537.']</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
@@ -3091,7 +3239,11 @@
           <t>["bs_stone@yahoo.com", "jeff@freeyellow.com", "Phillip.K.Allen@enron.com"]</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', '09/26/200011:57', 'AM', '---------------------------', 'Stone"&lt;bs_stone@yahoo.com&gt;', '09/26/200004:47:40', 'AM', '"jeff"&lt;jeff@freeyellow.com&gt;', '"PhillipKAllen"&lt;Phillip.K.Allen@enron.com&gt;', 'Phillip', '12noon', 'Brenda']</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
@@ -3142,7 +3294,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>['X37041', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
@@ -3236,7 +3392,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '09/25/200002:01PM', '---------------------------', 'Richard', 'Burchfield', 'Cindy', 'Cicchetti', '09/28/2000', '09/28/200002:00PM', '2537', 'Fletcher', 'JSturm/HOU/ECTScottNeal/HOU/ECTHunterSShively/HOU/ECTPhillipKAllen/HOU/ECTAllanSeverude/HOU/ECTScottMills/HOU/ECTRussSeverson/HOU/ECT', 'Burchfield/HOU/ECT', '09/28/2000', 'PM', 'Burchfield/HOU/ECT', 'JSturm/HOU/ECT(Invited)ScottNeal/HOU/ECT(Invited)HunterSShively/HOU/ECT(Invited)PhillipKAllen/HOU/ECT(Invited)AllanSeverude/HOU/ECT(Invited)ScottMills/HOU/ECT(Invited)RussSeverson/HOU/ECT(Invited)', '2537']</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
@@ -3317,7 +3477,11 @@
           <t>["Cindy Cicchetti", "Richard Burchfield", "Fletcher J Sturm", "Scott Neal", "Hunter S Shively", "Phillip K Allen", "Allan Severude", "Scott Mills", "Russ Severson"]</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '09/25/2000', '02:00PM', '---------------------------', 'Richard', 'Burchfield', 'Cindy', 'Cicchetti', '09/27/2000', '09/27/200002:00PM', '2537', 'Fletcher', 'Sturm/HOU/ECT', 'Scott', 'Neal/HOU/ECT', 'Hunter', 'SShively/HOU/ECT', 'KAllen/HOU/ECT', 'Allan', 'Severude/HOU/ECT', 'Scott', 'Mills/HOU/ECT', 'Severson/HOU/ECT']</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
@@ -3367,7 +3531,11 @@
           <t>["phone number"]</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>['Keith']</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
@@ -3405,7 +3573,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>['Mike', 'Grigsby', '37031', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
@@ -3452,7 +3624,11 @@
           <t>["Denver"]</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>['rockies', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -3486,7 +3662,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>['California', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -3591,7 +3771,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>['Keith', 'Westgate', 'Larry', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
@@ -3730,7 +3914,11 @@
           <t>["512-338-1110", "512-338-1103", "512-748-7495", "pallen@enron.com", "retwell@mail.sanmarcos.net", "cbpres@austin.rr.com", "george.richards@creeksidebuildersllc.com"]</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>['Phillip', '09/19/200004:35PM', '---------------------------', '"GeorgeRichards"&lt;cbpres@austin.rr.com&gt;', '09/08/200005:21:49AM', '&lt;cbpres@austin.rr.com&gt;', '"PhillipAllen"&lt;pallen@enron.com&gt;', 'Lewter"&lt;retwell@mail.sanmarcos.net&gt;', '28', 'North', 'St.Edwards', 'Westgate', 'Cameron', 'San', 'Larry', 'Lewter', 'SanAntonio', '512-338-1119', '512-338-1110.', '512-748-7495', '512-338-1103.', 'South', 'GeorgeW.Richards', 'Creekside']</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -3805,7 +3993,11 @@
           <t>["George", "Deborah Yates"]</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>['1308/1308', '2.7', 'Cherry', 'Deborah', 'Yates', 'De', 'Ville', 'Phillip', 'Allen']</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -3856,7 +4048,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
@@ -3894,7 +4090,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>['Brenda', 'Key', 'Stone', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
@@ -3938,7 +4138,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
@@ -3992,7 +4196,11 @@
           <t>["77845", "4303 Pate Rd.", "College Station"]</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>['August28th.', '4303', 'PateRd.', 'College', '77845.', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -4057,7 +4265,11 @@
           <t>["1406", "1410", "1411", "1415", "1416", "1417", "1425", "1428", "1438"]</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>['JulyAugust', '2929', '40854801', '581464', '318734282770', '1406', '1410', 'Crumps', 'Lucy', '1415', '1417,', '1425', '1428', "Ralph'sWhat", '1438', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -4140,7 +4352,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>['PhillipK', 'Allen/HOU/ECT', '09/12/2000', '11:22AM', '---------------------------', 'Michael', 'Etringer', '09/11/200002:32', 'PM', 'PhillipKAllen/HOU/ECT@ECT', 'market', 'Mike']</t>
+        </is>
+      </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
@@ -4178,7 +4394,11 @@
           <t>["pallen@enron.com"]</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>['http://www.hearme.com/vc2/?chnlOwnr=pallen@enron.com']</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
@@ -4252,7 +4472,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '05/02/2001', '05:26AM', '---------------------------', 'Ina', 'Rangel', '05/01/2001', '12:24PM', 'Phillip', 'PHILLIP', 'Phillip', 'Allen', 'pallenExtension:', '3-7041', 'EB3210C', 'INA', 'RANGEL']</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
@@ -4365,7 +4589,11 @@
           <t>["cbpres@austin.rr.com", "pallen@enron.com", "retwell@mail.sanmarcos.net", "512-338-1119", "512-338-1110", "512-748-7495", "512-338-1103"]</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>['Phillip', '09/11/200004:57PM', '---------------------------', '"GeorgeRichards"&lt;cbpres@austin.rr.com&gt;', '09/08/200005:21:49AM', '&lt;cbpres@austin.rr.com&gt;', '"PhillipAllen"&lt;pallen@enron.com&gt;', 'Lewter"&lt;retwell@mail.sanmarcos.net&gt;', '28', 'North', 'St.Edwards', 'Westgate', 'Cameron', 'San', 'Larry', 'Lewter', 'SanAntonio', '512-338-1119', '512-338-1110.', '512-748-7495', '512-338-1103.', 'South', 'GeorgeW.Richards', 'Creekside']</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
@@ -4405,7 +4633,11 @@
           <t>["San Marcos", "Friday evening", "Chelsea Villa", "Burnet deal"]</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>['SanMarcos', 'Burnet', 'Brenda', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
@@ -4460,7 +4692,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>['9/8', '9/7', '36,60037,200-600', 'NWPL', '-51,000-51,250', '250SanJuan-32,500-32,000-500', '9/8.', '300SanJuan']</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
@@ -4490,7 +4726,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>['aeco', 'NWPL', 'Nymex']</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
@@ -4528,7 +4768,11 @@
           <t>["sagewood", "Creekside"]</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>['2.7', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
@@ -4614,7 +4858,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '09/08/200012:29PM', '---------------------------', '"GeorgeRichards"&lt;cbpres@austin.rr.com&gt;', '09/08/200005:35:20AM', '&lt;cbpres@austin.rr.com&gt;', '"PhillipAllen"&lt;pallen@enron.com&gt;', 'Lewter"&lt;retwell@mail.sanmarcos.net&gt;,', 'Zuniga"&lt;invest@bga.com&gt;', 'Sagewood', 'Town', 'Homes', 'Regan', '1164/1302', 'psf', 'psf', 'Regan', 'George', 'W.', 'Richards', 'Creekside']</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
@@ -4723,7 +4971,11 @@
           <t>["pallen@enron.com","retwell@mail.sanmarcos.net","cbpres@austin.rr.com","512-338-1119","512-338-1110","512-748-7495","512-338-1103"]</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>['Phillip', '09/08/200012:28PM', '---------------------------', '"GeorgeRichards"&lt;cbpres@austin.rr.com&gt;', '09/08/200005:21:49AM', '&lt;cbpres@austin.rr.com&gt;', '"PhillipAllen"&lt;pallen@enron.com&gt;', 'Lewter"&lt;retwell@mail.sanmarcos.net&gt;', '28', 'North', 'St.Edwards', 'Westgate', 'Cameron', 'San', 'Larry', 'Lewter', 'SanAntonio', '512-338-1119', '512-338-1110.', '512-748-7495', '512-338-1103.', 'South', 'GeorgeW.Richards', 'Creekside']</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
@@ -4770,7 +5022,11 @@
           <t>["stagecoachmama@hotmail.com", "pallen@enron.com"]</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '09/06/2000', '03:53PM', '---------------------------', '"LucyGonzalez"&lt;stagecoachmama@hotmail.com&gt;', '09/06/2000', '09:06:45AM', 'pallen@enron.com', '_________________________________________________________________________', 'http://www.hotmail.com.', 'http://profiles.msn.com.']</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
@@ -4859,7 +5115,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '09/06/200002:01PM', '---------------------------', 'Enron-admin@FSDDataSvc.com', '09/06/2000', '10:12:33AM', 'pallen@enron.com', 'Manager', 'Thursday,September', 'http://www.fsddatasvc.com/enron', 'EVH3JY', 'Shively', 'Dennis', 'Ward', '713-942-8436.', 'Debbie', 'Nowak', '713-853-3304,', 'Christi', 'Smith', 'Keilty,Goldsmith&amp;', '858-450-2554.']</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
@@ -4907,7 +5167,11 @@
           <t>["Reagan Lehmann", "1308"]</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>['sagewood', 'Reagan', 'Reagan', '1308', 'million', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
@@ -5173,7 +5437,11 @@
 Overall, this email aims to inform users about the availability of OWA as a temporary solution until their Outlook client is configured on their desktop.</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '05/01/20010=2:14PM', '---------------------------', '04/27/200101:01PM', 'Horton/NA/Enron@ENRON,', 'Baig/NA/Enron@ENRON,', 'Brandon', 'Bang=erter/NA/Enron@Enron,', 'BrianEllis/Corp/Enron@Enron,', 'p/Enron@ENRON,', 'Wood/NA/Enron@Enron,ChrisTull/HOU/ECT@ECT,Dale', 'Sm=ith/Corp/Enron@ENRON,', 'Dave', 'June/NA/Enron@ENRON,', 'Sutton/NA/Enron@Enro=n,', 'Buenrostro/HR/Corp/Enron@ENRON,', 'Morrison/Corp/Enron@ENRON=,', 'Dorn/Corp/Enron@ENRON,', 'Schultea/HR/Corp/Enron@ENRON,', 'McD=', 'owell/NA/Enron@ENRON,', 'Barrios/Corp/Enron@ENRON,', 'Brown/HR/Cor=p/Enron@ENRON,', 'Perubhatla/Corp/Enron@Enron,', 'Shekar', 'Komatireddy/NA/Enron=@Enron,', 'Yowman/Corp/Enron@ENRON,', "AngieO'Brian/HR/Corp/Enron@ENRON,=", 'Castellano/HR/Corp/Enron@ENRON,', 'Gorsuch/NA/Enron@ENRON,', 'LaQuitta', 'Washington/HR/Corp/Enron@ENRON,', 'son/HR/Corp/Enron@ENRON,', 'Lighthill/HR/Corp/Enron@ENRON,', 'Ho=pe/HOU/ECT@ECT,', 'CharlotteBrown/HR/Corp/Enron@ENRON,RonaldFain/HR/Corp/En=ron@ENRON,GaryFitch/HR/Corp/Enron@Enron,AnnaHarris/HR/Corp/Enron@ENRON,=KeithJones/HR/Corp/Enron@ENRON,', 'Monson/NA/Enron@Enron,', 'el/HR/Corp/Enron@ENRON,JohnStabler/HR/Corp/Enron@ENRON,Michelle', 'Prince/N=A/Enron@Enron,', 'JamesGramke/NA/Enron@ENRON,BlairHicks/NA/Enron@ENRON,', 'Lit=tle/Enron@EnronXGate,', 'DaleLukert/NA/Enron@ENRON,DonaldMartin/NA/Enron@EN=RON,Andrew', 'Mattei/NA/Enron@ENRON,', 'DarvinMitchell/NA/Enron@ENRON,Mark', 'Old=ham/NA/Enron@ENRON,', 'Pearson/NA/Enron@ENRON,', 'Rau/NA/Enron@ENRON,', 'WilliamRedick/NA/En=ron@ENRON,', 'ARichardson/NA/Enron@ENRON,', 'Schnieders/NA/Enron@ENR=ON,', 'Simmons/NA/Enron@Enron,', 'Trimble/NA/Enron@ENRON,David', 'MikeBoegler/HR/Corp/Enron@ENRON,Lyndel', 'Click/HR/Corp/En=ron@ENRON,', 'Franco/NA/Enron@Enron,', 'RandyGross/HR/Corp/Enron@Enron,=ArthurJohnson/HR/Corp/Enron@Enron,DannyJones/HR/Corp/Enron@ENRON,', 'gden/Houston/Eott@Eott,', 'Ponce/NA/Enron@Enron,', 'TracyPursifull/HR/Corp=/Enron@ENRON,LanceStanley/HR/Corp/Enron@ENRON,FrankErmis/HOU/ECT@ECT,', 'JayReitmeyer/HOU/ECT@ECT,KeithHolst/HOU/ECT@ect=,MatthewLenhart/HOU/ECT@ECT,MikeGrigsby/HOU/ECT@ECT,Monique', 'U/ECT@ECT,', 'KAllen/HOU/ECT@ECT,RandallLGay/HOU/ECT@ECT,', 'Kuy=kendall/HOU/ECT@ECT,', 'HFletcher/HOU/ECT@ECT,', 'Wukasch/Corp/Enr=on@ENRON,', 'Franklin/HOU/ECT@ECT,MikePotter/NA/Enron@Enron,', 'Na=talie', 'Baker/HOU/ECT@ECT,', 'Calcagno/NA/Enron@Enron,', 'rp/Enron@Enron,', 'Franklin/Corp/Enron@ENRON,', 'Villarreal/HOU/ECT=@ECT,JoanCollins/HOU/EES@EES,JoeACasas/HOU/ECT@ECT,', 'Loocke/ENRON=@enronXgate,', 'Halstead/NA/Enron@ENRON,', 'Meredith', 'Homco/HOU/ECT@ECT,', 'Rober=t', 'Allwein/HOU/ECT@ECT,', 'ScottLoving/NA/Enron@ENRON,', 'Boudreaux/ENRON@=enronXgate,', 'Gillespie/Corp/Enron@ENRON,', 'Carter/NA/Enron@ENRON,=', 'Wood/NA/Enron@ENRON,', 'Fuzat/Enron', 'Netek/Enron', 'NA/Enron@Enron,', 'Gerard/Corp/Enron@ENRON,', 'Taylor/HOU/ECT@ECT,=', 'Hangach/NYC/MGUSA@MGUSA,', 'Gagel/NYC/MGUSA@MGUSA,', 'NYC/MGUSA@MGUSA,', 'Balladares/NYC/MGUSA@MGUSA,', 'Strutt/NYC/MGUSA@MGUS=', 'ma=il', 'http://nahou=-msowa01p/exchange/john.doe', '=09Outlook.2000@enron.com', '=09713-853-1411']</t>
+        </is>
+      </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
@@ -5202,7 +5470,11 @@
           <t>["Jean Mrha"]</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>['Ina,', 'Jean', 'Mrha', '3:30']</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
@@ -5480,7 +5752,11 @@
 Note: The word "data" and "center" are actually referring to the same thing, but I've counted them separately since they're used in different contexts throughout the text.</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '09/06/2000', '10:49AM', '---------------------------', '09/06/200007:39AM', 'Phillip', 'Richter/HOU/ECT', '09/06/2000', '09:45AM', '---------------------------', 'Swerzbin/HOU/ECT@ECT,RobertBadeer/HOU/ECT@ECT,SeanCrandall/PDX/ECT@ECT,TimBelden/HOU/ECT@ECT,JeffRichter/HOU/ECT@ECT,JohnMForney/HOU/ECT@ECT,MattMotley/PDX/ECT@ECT,TomAlonso/PDX/ECT@ECT,MarkFischer/PDX/ECT@ECT', 'Belden/HOU/ECT', '09/06/200007:27', 'AM', '---------------------------', 'KevinM', 'Presto', '09/05/200001:59PM', 'Belden/HOU/ECT@ECT', 'Herndon/HOU/ECT@ect,JohnZufferli/HOU/ECT@ECT,LloydWill/HOU/ECT@ECT,', 'Gilbert-Smith/Corp/Enron@ENRON,', 'Swerzbin/HOU/ECT@ECT', 'Porltand,Boise,Denver,', 'SanFran', 'and', 'SanJose', 'KevinM', 'Presto/HOU/ECT', '09/05/200003:41PM', '---------------------------', 'America', 'John', 'Suarez', '09/05/200001:45PM', 'MPresto/HOU/ECT@ECT,', 'DanaDavis/HOU/ECT@ECT,', 'JBroderick/HOU/ECT@ECT,', 'Miller/NA/Enron@Enron', 'John', 'Suarez/HOU/ECT', '09/05/2000', '01:46PM', '---------------------------', 'Hopley', '09/05/2000', '11:41AM', 'John', 'Suarez/HOU/ECT@ECT,', 'Suresh', 'Vasan/Enron', 'September05,2000', 'Tukwila.', 'AboveNet,GlobixandHostPro', 'Tukwila', 'KentValley', 'Southcenter', 'Karl', 'Karzmar,', 'manager', 'Karzmar', 'Bob', 'Royer,', 'director', 'Tukwila', 'SabeyCorp.', 'Laurent', 'ICGCommunications,NetStreamCommunications,PacWestTelecommandZamaNetworks', 'Tukwila', 'Steve']</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
@@ -5524,7 +5800,11 @@
           <t>["Tori K.", "Martin Cuilla", "Phillip K Allen", "John J Lavorato"]</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>['Ina,', 'H.R.----------------------', 'Phillip', 'Allen/HOU/ECT', '09/06/2000', '10:44AM', '---------------------------', 'JohnJ', '09/06/200005:39AM', 'Phillip', 'Allen/HOU/ECT@ECT', 'Hunter']</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
@@ -5546,7 +5826,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
@@ -5656,7 +5940,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>['Phillip', '09/05/200001:50PM', '---------------------------', '"ChristiSmith"&lt;christi.smith@lrinet.com&gt;', '09/05/200011:40:59AM', '&lt;christi.smith@lrinet.com&gt;', '&lt;Phillip.K.Allen@enron.com&gt;', 'Nowak', '&lt;dnowak@enron.com&gt;', 'Christi', 'Christi', 'Smith', '[mailto:christi.smith@lrinet.com]', 'Thursday,August31,2000', '10:33AM', "'Phillip.K.Allen@enron.com'", 'Debbie', 'Nowak', 'Deborah', 'Evans', 'Phillip.ChristiL.Smith', 'Keilty,Goldsmith&amp;Company', '858/450-2554', 'PhillipKAllen[mailto:Phillip.K.Allen@enron.com]', 'Thursday,August31,2000', 'PM', 'debe@fsddatasvc.com', 'Holst-D', 'Ermis-D', 'South-D', 'Tholt-D', 'Neal-P', 'Shively-P', 'Martin-P', 'Arnold-P']</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
@@ -5699,7 +5987,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '09/05/2000', '01:29PM', '---------------------------', 'PhillipK', 'Allen', '08/29/200002:20PM', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
@@ -5745,7 +6037,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '09/01/200001:07PM', '---------------------------', 'NorthAmerica', 'Matt', 'Motley', '09/01/200008:53AM', 'PhillipKAllen/HOU/ECT@ECT', 'Ray', 'Niles']</t>
+        </is>
+      </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
@@ -5778,7 +6074,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>['california']</t>
+        </is>
+      </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
@@ -5810,7 +6110,11 @@
           <t>["Jay Reitmeyer"]</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>['newwestpower', 'Jay', 'Reitmeyer.', 'analyst', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
@@ -5907,7 +6211,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '08/31/200001:13', 'PM', '---------------------------', '"ChristiSmith"&lt;christi.smith@lrinet.com&gt;', '08/31/200010:32:49AM', '&lt;christi.smith@lrinet.com&gt;', '&lt;Phillip.K.Allen@enron.com&gt;', 'Nowak', '&lt;dnowak@enron.com&gt;,', '"DeborahEvans', '&lt;debe@fsddatasvc.com&gt;', 'Phillip.ChristiL.Smith', 'Keilty,Goldsmith&amp;Company', '858/450-2554', 'PhillipKAllen[mailto:Phillip.K.Allen@enron.com]', 'Thursday,August31,2000', '12:03PM', 'debe@fsddatasvc.com', 'Holst-D', 'Ermis-D', 'South-D', 'Tholt-D', 'Neal-P', 'Shively-P', 'Martin-P', 'Arnold-P']</t>
+        </is>
+      </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
@@ -6147,7 +6455,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '05/01/20010=2:14PM', '---------------------------', '04/27/200101:00PM', 'Horton/NA/Enron@ENRON,', 'Baig/NA/Enron@ENRON,', 'Bang=erter/NA/Enron@Enron,', 'BrianEllis/Corp/Enron@Enron,', 'p/Enron@ENRON,', 'ChrisTull/HOU/ECT@ECT,', 'Sm=ith/Corp/Enron@ENRON,', 'June/NA/Enron@ENRON,', 'Buenrostro/HR/Corp/Enron@ENRON,', 'Morrison/Corp/Enron@ENRON=', 'Dorn/Corp/Enron@ENRON,', 'Schultea/HR/Corp/Enron@ENRON,', 'McD=owell/NA/Enron@ENRON,', 'Barrios/Corp/Enron@ENRON,', 'Brown/HR/Cor=p/Enron@ENRON,', 'Perubhatla/Corp/Enron@Enron,', 'Shekar', 'Komatireddy/NA/Enron=@Enron,', 'Yowman/Corp/Enron@ENRON,', "O'Brian/HR/Corp/Enron@ENRON,", 'Castellano/HR/Corp/Enron@ENRON,', 'Gorsuch/NA/Enron@ENRON,', 'Jo', '=Matson/Corp/Enron@ENRON,', 'LaQuitta', 'Washington/HR/Corp/Enron@ENRON,', 'son/HR/Corp/Enron@ENRON,', 'Lighthill/HR/Corp/Enron@ENRON,', 'Ho=pe/HOU/ECT@ECT,', 'Brown/HR/Corp/Enron@ENRON,', 'Fain/HR/Corp/En=', 'ron@ENRON,GaryFitch/HR/Corp/Enron@Enron,', 'Harris/HR/Corp/Enron@ENRON,=KeithJones/HR/Corp/Enron@ENRON,', 'Monson/NA/Enron@Enron,', 'McNi=el/HR/Corp/Enron@ENRON,', 'Stabler/HR/Corp/Enron@ENRON,', 'Prince/N=A/Enron@Enron,', 'Gramke/NA/Enron@ENRON,', 'Hicks/NA/Enron@ENRON,', 'Lit=tle/Enron@EnronXGate,', 'Lukert/NA/Enron@ENRON,', 'Martin/NA/Enron@EN=', 'RON,', 'Mattei/NA/Enron@ENRON,', 'DarvinMitchell/NA/Enron@ENRON,', 'Old=ham/NA/Enron@ENRON,', 'Pearson/NA/Enron@ENRON,', 'Rau/NA/Enron@ENRON,', 'Redick/NA/En=ron@ENRON,', 'ARichardson/NA/Enron@ENRON,', 'Schnieders/NA/Enron@ENR=ON,', 'Simmons/NA/Enron@Enron,', 'Trimble/NA/Enron@ENRON,', 'Boegler/HR/Corp/Enron@ENRON,', 'Click/HR/Corp/En=ron@ENRON,', 'Franco/NA/Enron@Enron,', 'RandyGross/HR/Corp/Enron@Enron,=ArthurJohnson/HR/Corp/Enron@Enron,DannyJones/HR/Corp/Enron@ENRON,', 'gden/Houston/Eott@Eott,', 'Ponce/NA/Enron@Enron,', 'Pursifull/HR/Corp=', '/Enron@ENRON,', 'Stanley/HR/Corp/Enron@ENRON,', 'Ermis/HOU/ECT@ECT,', 'Reitmeyer/HOU/ECT@ECT,KeithHolst/HOU/ECT@ect=,MatthewLenhart/HOU/ECT@ECT,MikeGrigsby/HOU/ECT@ECT,', 'U/ECT@ECT,', 'KAllen/HOU/ECT@ECT,', 'LGay/HOU/ECT@ECT,', 'Kuy=kendall/HOU/ECT@ECT,', 'Fletcher/HOU/ECT@ECT,', 'Wukasch/Corp/Enr=on@ENRON,', 'Franklin/HOU/ECT@ECT,', 'Potter/NA/Enron@Enron,', 'Na=talie', 'Baker/HOU/ECT@ECT,', 'Calcagno/NA/Enron@Enron,', 'rp/Enron@Enron,', 'Franklin/Corp/Enron@ENRON,', 'Villarreal/HOU/ECT=@ECT,', 'Collins/HOU/EES@EES,', 'A', 'Casas/HOU/ECT@ECT,', 'Loocke/ENRON=@enronXgate,', 'Halstead/NA/Enron@ENRON,', 'Homco/HOU/ECT@ECT,', 'Allwein/HOU/ECT@ECT,', 'Loving/NA/Enron@ENRON,', 'Boudreaux/ENRON@=enronXgate,', 'Gillespie/Corp/Enron@ENRON,', 'Carter/NA/Enron@ENRON,=', 'Wood/NA/Enron@ENRON,', 'Fuzat/Enron', 'Netek/Enron', 'NA/Enron@Enron,', 'Gerard/Corp/Enron@ENRON,', 'Taylor/HOU/ECT@ECT,', 'Hangach/NYC/MGUSA@MGUSA,', 'Gagel/NYC/MGUSA@MGUSA,', 'NYC/MGUSA@MGUSA,', 'Balladares/NYC/MGUSA@MGUSA,', 'Strutt/NYC/MGUSA@MGUS=', '---------------------------------------------------------------------------=-----------------------------------------------------------------']</t>
+        </is>
+      </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
@@ -6191,7 +6503,11 @@
           <t>["Mike Grigsby", "Keith Holst", "Frank Ermis", "Steve South", "Janie Tholt", "Hunter Shively", "Tom Martin", "John Arnold"]</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>['Holst-D', 'Ermis-D', 'South-D', 'Tholt-D', 'Neal-P', 'Shively-P', 'Martin-P', 'Arnold-P']</t>
+        </is>
+      </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
@@ -6233,7 +6549,11 @@
           <t>["phillip k allen", "08/29/2000 02:20 pm", "mark@intelligencepress.com"]</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '08/31/2000', '10:17AM', '---------------------------', 'PhillipK', 'Allen', '08/29/200002:20PM', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
@@ -6269,7 +6589,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>['Keith']</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
@@ -6291,7 +6615,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
@@ -6322,7 +6650,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr"/>
@@ -6354,7 +6686,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>['enron', 'socal', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
@@ -6387,7 +6723,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>['Brenda', 'College', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
@@ -6461,7 +6801,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>['----------------------', 'PhillipK', 'Allen/HOU/ECT', '08/28/2000', '01:39PM', '---------------------------', 'KristianJ', 'Lande', '08/24/200003:56', 'PM', 'ChristopherF', 'Calger/PDX/ECT@ECT,', 'Thomas/HOU/ECT@ECT,', 'WVickers/HOU/ECT@ECT,ElliotMainzer/PDX/ECT@ECT,MichaelMcDonald/SF/ECT@ECT,DavidParquet/SF/ECT@ECT,LairdDyer/SF/ECT@ECT,JimBuerkle/PDX/ECT@ECT,JimGilbert/PDX/ECT@ECT,', 'WDonovan/HOU/ECT@ECT,', 'Clark/PDX/ECT@ECT', 'Belden/HOU/ECT@ECT,', 'Badeer/HOU/ECT@ECT,', 'Motley/PDX/ECT@ECT,', 'Allen/HOU/ECT@ECT', 'August24,2000']</t>
+        </is>
+      </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
@@ -6513,7 +6857,11 @@
           <t>["GNA45925", "YJ53KU42", "713", "4357"]</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>['GNA45925', 'YJ53KU42', 'www.enrononline.com', 'western', '(713)853-7041', 'Kathy', '713/853-HELP(4357).', 'Phillip', 'Allen']</t>
+        </is>
+      </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
@@ -6570,7 +6918,11 @@
           <t>["Enron", "Socal", "San Juan", "Socal Index", "Gas Daily"]</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>['socalbasis', 'socal/sanjuan', 'Juan', '4.91', 'Juan', '1.04', '.99', '4.49', 'Enron', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
@@ -6600,7 +6952,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>['Keith', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
@@ -6631,7 +6987,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
@@ -6662,7 +7022,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr"/>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>['Mike', 'Grigsby', 'Patti', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
@@ -6706,7 +7070,11 @@
           <t>["john.lavorato@enron.com", "hunter.shively@enron.com"]</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>['john.lavorato@enron.com,hunter.shively@enron.com', 'john.lavorato@enron.com,hunter.shively@enron.com', 'Tori', 'Kuykendall,', 'commercialsupportmanager', 'Martin', 'Cuilla', 'Tori.Hunter', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
@@ -6735,7 +7103,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
@@ -6774,7 +7146,11 @@
           <t>["amount owed", "amount paid"]</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr"/>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
@@ -6804,7 +7180,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>['Phillip']</t>
+        </is>
+      </c>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="inlineStr"/>
@@ -6826,7 +7206,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr"/>
@@ -6859,7 +7243,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr"/>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>['2:00.', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr"/>
@@ -6887,7 +7275,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
@@ -6918,7 +7310,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr"/>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
@@ -6992,7 +7388,11 @@
 ]</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>['----------------------', 'Phillip', 'Allen/HOU/ECT', '04/30/200111:21AM', '---------------------------', 'Comnes', '04/27/200101:38PM', 'Joe', 'Hartsoe/Corp/Enron@ENRON', 'Steve', 'Kean', 'Kean/Lay', 'Alan', 'Comnes', 'Comnes/PDX/ECT', '04/27/200101:42PM', '---------------------------', 'Janel', '04/27/200112:44PM', 'Comnes/PDX/ECT@ECT,', 'Jeff', 'Dasovich/NA/Enron@Enron', 'Kaufman/PDX/ECT@ECT,', 'Richard', 'Shapiro/NA/Enron@Enron', 'Steve', 'Kean', 'Lay']</t>
+        </is>
+      </c>
       <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
@@ -7055,7 +7455,11 @@
           <t>["$985,721,000", "$1.00", "116,897,000", "$2.95", "$2.86", "$10", "34", "37", "81", "SLB", "Calpine", "Tosco"]</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>['334,340,000/year', '(334,340,000', 'mct', 'X', '37', 'Gas', '34', '10', 'Calpine,Tosco,andSLB?', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
@@ -7112,7 +7516,11 @@
           <t>["lucy Gonzalez", "pallen@enron.com", "wade", "mary", "28", "25", "hotmail", "stagecoachmama"]</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '08/20/200005:39PM', '---------------------------', '"LucyGonzalez"&lt;stagecoachmama@hotmail.com&gt;', '08/15/200002:32:57PM', 'pallen@enron.com', 'Wade', 'Lucy', '________________________________________________________________________', 'http://www.hotmail.com']</t>
+        </is>
+      </c>
       <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="inlineStr"/>
@@ -7182,7 +7590,11 @@
           <t>["stagecoachmama@hotmail.com", "pallen@enron.com"]</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '08/20/2000', '05:38PM', '---------------------------', '"LucyGonzalez"&lt;stagecoachmama@hotmail.com&gt;', '08/16/2000', '02:44:36PM', 'pallen@enron.com', 'pd', '8/16/00', '8/15/00', '(frig=125.00)DELCHRG=15.00\\TAX=18.56', 'CK', '1427=108.25', 'sTEELMANOFFICE', 'Lucy', '________________________________________________________________________', 'http://www.hotmail.com']</t>
+        </is>
+      </c>
       <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
@@ -7232,7 +7644,11 @@
           <t>[{"hotmail", "stagecoachmama"}, {"enron", "pallen"}, {"yahoo", "msn"}]</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr"/>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>['Phillip', 'Allen/HOU/ECT', '08/20/200005:38', 'PM', '---------------------------', '"LucyGonzalez"&lt;stagecoachmama@hotmail.com&gt;', '08/17/2000', '02:37:55PM', 'pallen@enron.com', 'gary', 'Lucy', '________________________________________________________________________', 'http://www.hotmail.com']</t>
+        </is>
+      </c>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
@@ -7270,7 +7686,11 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr"/>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>['Smith', 'Paine', 'JDSU', 'SDLI?', 'Phillip']</t>
+        </is>
+      </c>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>

</xml_diff>